<commit_message>
Alteração nos artefatos de Qualidade.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Registro de Não Conformidade.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Registro de Não Conformidade.xlsx
@@ -40,9 +40,6 @@
     <t>Produto/Processo</t>
   </si>
   <si>
-    <t>Severidade</t>
-  </si>
-  <si>
     <t>Legenda Status</t>
   </si>
   <si>
@@ -50,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Registro de Não Conformidades do Projeto EveRemind</t>
+  </si>
+  <si>
+    <t>Criticidade</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -524,7 +526,7 @@
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="10"/>
@@ -539,7 +541,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -581,7 +583,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="I5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1">
@@ -605,7 +607,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="I7" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
[GQA] Atualização do registro de NC.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Registro de Não Conformidade.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Registro de Não Conformidade.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Registro de Não Conformidades" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Data de Abertura</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Casos de Teste (Planejamento 1)</t>
+  </si>
+  <si>
+    <t>Solucionada</t>
   </si>
 </sst>
 </file>
@@ -118,7 +121,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,8 +164,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -198,11 +207,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,6 +271,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -549,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
@@ -612,7 +641,7 @@
       <c r="E3" s="13">
         <v>42158</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="10"/>
@@ -633,10 +662,12 @@
       <c r="E4" s="13">
         <v>42159</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="11"/>
+      <c r="F4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="13">
+        <v>42157</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
@@ -660,10 +691,12 @@
       <c r="E5" s="13">
         <v>42160</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="11"/>
+      <c r="F5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="13">
+        <v>42158</v>
+      </c>
       <c r="I5" s="8" t="s">
         <v>3</v>
       </c>
@@ -687,10 +720,12 @@
       <c r="E6" s="13">
         <v>42159</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="11"/>
+      <c r="F6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="13">
+        <v>42157</v>
+      </c>
       <c r="I6" s="9" t="s">
         <v>8</v>
       </c>
@@ -704,8 +739,11 @@
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="11"/>
+      <c r="I7" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="11"/>

</xml_diff>

<commit_message>
[GQA] Atualização no Registro de NC.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Registro de Não Conformidade.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Registro de Não Conformidade.xlsx
@@ -258,9 +258,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -289,6 +286,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -588,7 +588,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
@@ -635,172 +635,174 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>42154</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>42158</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="10"/>
+      <c r="F3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="20">
+        <v>42161</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>42154</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>42159</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>42157</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>42154</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>42160</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>42158</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <v>42154</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>42159</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>42157</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="11"/>
-      <c r="I7" s="19" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="10"/>
+      <c r="I7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>